<commit_message>
styling looking much better, sample results updated
</commit_message>
<xml_diff>
--- a/sample_results.xlsx
+++ b/sample_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrew/Library/Mobile Documents/com~apple~CloudDocs/Code/projects/kahootmate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C4C5058-ABC8-7B4E-9006-BBB42374D377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99270101-C41F-4F44-903A-70787210F56E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17100" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="116">
   <si>
     <t>Played on</t>
   </si>
@@ -216,9 +216,6 @@
     <t>apalacci03</t>
   </si>
   <si>
-    <t>2 players</t>
-  </si>
-  <si>
     <t>3 of 3</t>
   </si>
   <si>
@@ -315,10 +312,73 @@
     <t>31.96%</t>
   </si>
   <si>
-    <t>Jim</t>
-  </si>
-  <si>
-    <t>Jack</t>
+    <t>Andrew</t>
+  </si>
+  <si>
+    <t>Eyob</t>
+  </si>
+  <si>
+    <t>Liz</t>
+  </si>
+  <si>
+    <t>Shahara</t>
+  </si>
+  <si>
+    <t>Becca</t>
+  </si>
+  <si>
+    <t>Alia</t>
+  </si>
+  <si>
+    <t>Algebra II Review Kahoot</t>
+  </si>
+  <si>
+    <t>21 players</t>
+  </si>
+  <si>
+    <t>Ivelisse</t>
+  </si>
+  <si>
+    <t>Justin</t>
+  </si>
+  <si>
+    <t>Tre</t>
+  </si>
+  <si>
+    <t>Lique</t>
+  </si>
+  <si>
+    <t>Evetty</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>Dylan</t>
+  </si>
+  <si>
+    <t>Kelly</t>
+  </si>
+  <si>
+    <t>Robin</t>
+  </si>
+  <si>
+    <t>Leo</t>
+  </si>
+  <si>
+    <t>Tiger</t>
+  </si>
+  <si>
+    <t>Jean</t>
+  </si>
+  <si>
+    <t>Sam</t>
+  </si>
+  <si>
+    <t>Ethan</t>
+  </si>
+  <si>
+    <t>Gregor</t>
   </si>
 </sst>
 </file>
@@ -688,7 +748,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
@@ -785,42 +845,42 @@
     <xf numFmtId="49" fontId="17" fillId="17" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="3" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
@@ -833,41 +893,44 @@
     <xf numFmtId="49" fontId="4" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="15" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="13" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="14" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="13" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="14" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="15" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1254,7 +1317,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="A11" sqref="A11:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.375" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -1270,130 +1333,130 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
+      <c r="A1" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
     </row>
     <row r="2" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
     </row>
     <row r="3" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
     </row>
     <row r="4" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="33" t="s">
-        <v>61</v>
-      </c>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
+      <c r="B4" s="43" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
     </row>
     <row r="5" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="33" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
+      <c r="B5" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="34"/>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
+      <c r="A6" s="32"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
     </row>
     <row r="7" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="35"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
     </row>
     <row r="8" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="36" t="s">
+      <c r="A8" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="36"/>
-      <c r="C8" s="37">
+      <c r="B8" s="34"/>
+      <c r="C8" s="41">
         <v>0.3333333432674408</v>
       </c>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
     </row>
     <row r="9" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="36"/>
-      <c r="C9" s="37">
+      <c r="B9" s="34"/>
+      <c r="C9" s="41">
         <v>0.66666668653488159</v>
       </c>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="37"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
     </row>
     <row r="10" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="36" t="s">
+      <c r="A10" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="36"/>
+      <c r="B10" s="34"/>
       <c r="C10" s="38">
-        <v>846</v>
+        <v>590.95000000000005</v>
       </c>
       <c r="D10" s="38"/>
       <c r="E10" s="38"/>
@@ -1402,92 +1465,92 @@
       <c r="H10" s="38"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="34"/>
-      <c r="B11" s="34"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
     </row>
     <row r="12" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="35"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
     </row>
     <row r="13" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="36" t="s">
+      <c r="A13" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="36"/>
-      <c r="C13" s="39">
-        <v>0</v>
-      </c>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="40">
+        <v>0</v>
+      </c>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
     </row>
     <row r="14" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="36" t="s">
+      <c r="A14" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="36"/>
-      <c r="C14" s="40">
-        <v>0</v>
-      </c>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="37">
+        <v>0</v>
+      </c>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
     </row>
     <row r="15" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="36"/>
-      <c r="C15" s="41">
-        <v>0</v>
-      </c>
-      <c r="D15" s="41"/>
-      <c r="E15" s="42">
-        <v>0</v>
-      </c>
-      <c r="F15" s="42"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="40"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="35">
+        <v>0</v>
+      </c>
+      <c r="D15" s="35"/>
+      <c r="E15" s="36">
+        <v>0</v>
+      </c>
+      <c r="F15" s="36"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
     </row>
     <row r="16" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="36" t="s">
+      <c r="A16" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="36"/>
-      <c r="C16" s="41">
-        <v>0</v>
-      </c>
-      <c r="D16" s="41"/>
-      <c r="E16" s="42">
-        <v>0</v>
-      </c>
-      <c r="F16" s="42"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="35">
+        <v>0</v>
+      </c>
+      <c r="D16" s="35"/>
+      <c r="E16" s="36">
+        <v>0</v>
+      </c>
+      <c r="F16" s="36"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
     </row>
     <row r="17" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="36" t="s">
+      <c r="A17" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="36"/>
+      <c r="B17" s="34"/>
       <c r="C17" s="5" t="s">
         <v>14</v>
       </c>
@@ -1508,29 +1571,52 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="34"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
+      <c r="A18" s="32"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
     </row>
     <row r="19" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="43"/>
-      <c r="C19" s="43"/>
-      <c r="D19" s="43"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="43"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="A7:H7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:H8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:H9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="A12:H12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:H13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
     <mergeCell ref="A18:H18"/>
     <mergeCell ref="A19:H19"/>
     <mergeCell ref="A16:B16"/>
@@ -1538,29 +1624,6 @@
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C14:H14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:H10"/>
-    <mergeCell ref="A11:H11"/>
-    <mergeCell ref="A12:H12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:H13"/>
-    <mergeCell ref="A6:H6"/>
-    <mergeCell ref="A7:H7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:H8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:H9"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="B5:H5"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1573,10 +1636,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8893CFB2-DE85-214E-95E1-BD5AE6AFB100}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.125" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -1588,13 +1651,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
+      <c r="A1" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
       <c r="F1" s="44"/>
     </row>
     <row r="2" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1629,10 +1692,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="C4" s="23">
-        <v>956</v>
+        <v>93</v>
+      </c>
+      <c r="C4" s="60">
+        <v>983</v>
       </c>
       <c r="D4" s="23">
         <v>1</v>
@@ -1649,10 +1712,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="C5" s="23">
-        <v>736</v>
+        <v>94</v>
+      </c>
+      <c r="C5" s="60">
+        <v>972</v>
       </c>
       <c r="D5" s="23">
         <v>1</v>
@@ -1661,6 +1724,386 @@
         <v>2</v>
       </c>
       <c r="F5" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="23">
+        <v>3</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="60">
+        <v>921</v>
+      </c>
+      <c r="D6" s="23">
+        <v>1</v>
+      </c>
+      <c r="E6" s="23">
+        <v>2</v>
+      </c>
+      <c r="F6" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="23">
+        <v>4</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7" s="60">
+        <v>874</v>
+      </c>
+      <c r="D7" s="23">
+        <v>1</v>
+      </c>
+      <c r="E7" s="23">
+        <v>2</v>
+      </c>
+      <c r="F7" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="23">
+        <v>5</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" s="60">
+        <v>835</v>
+      </c>
+      <c r="D8" s="23">
+        <v>1</v>
+      </c>
+      <c r="E8" s="23">
+        <v>2</v>
+      </c>
+      <c r="F8" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="23">
+        <v>6</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="C9" s="60">
+        <v>801</v>
+      </c>
+      <c r="D9" s="23">
+        <v>1</v>
+      </c>
+      <c r="E9" s="23">
+        <v>2</v>
+      </c>
+      <c r="F9" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="23">
+        <v>7</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" s="60">
+        <v>745</v>
+      </c>
+      <c r="D10" s="23">
+        <v>1</v>
+      </c>
+      <c r="E10" s="23">
+        <v>2</v>
+      </c>
+      <c r="F10" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="23">
+        <v>8</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="C11" s="60">
+        <v>721</v>
+      </c>
+      <c r="D11" s="23">
+        <v>1</v>
+      </c>
+      <c r="E11" s="23">
+        <v>2</v>
+      </c>
+      <c r="F11" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="23">
+        <v>9</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="C12" s="60">
+        <v>704</v>
+      </c>
+      <c r="D12" s="23">
+        <v>1</v>
+      </c>
+      <c r="E12" s="23">
+        <v>2</v>
+      </c>
+      <c r="F12" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="23">
+        <v>10</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="C13" s="60">
+        <v>643</v>
+      </c>
+      <c r="D13" s="23">
+        <v>1</v>
+      </c>
+      <c r="E13" s="23">
+        <v>2</v>
+      </c>
+      <c r="F13" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="23">
+        <v>11</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="C14" s="60">
+        <v>631</v>
+      </c>
+      <c r="D14" s="23">
+        <v>1</v>
+      </c>
+      <c r="E14" s="23">
+        <v>2</v>
+      </c>
+      <c r="F14" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="23">
+        <v>12</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="C15" s="60">
+        <v>581</v>
+      </c>
+      <c r="D15" s="23">
+        <v>1</v>
+      </c>
+      <c r="E15" s="23">
+        <v>2</v>
+      </c>
+      <c r="F15" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="23">
+        <v>13</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="C16" s="60">
+        <v>519</v>
+      </c>
+      <c r="D16" s="23">
+        <v>1</v>
+      </c>
+      <c r="E16" s="23">
+        <v>2</v>
+      </c>
+      <c r="F16" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="23">
+        <v>14</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="C17" s="60">
+        <v>483</v>
+      </c>
+      <c r="D17" s="23">
+        <v>1</v>
+      </c>
+      <c r="E17" s="23">
+        <v>2</v>
+      </c>
+      <c r="F17" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="23">
+        <v>15</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="C18" s="60">
+        <v>425</v>
+      </c>
+      <c r="D18" s="23">
+        <v>1</v>
+      </c>
+      <c r="E18" s="23">
+        <v>2</v>
+      </c>
+      <c r="F18" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="23">
+        <v>16</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="C19" s="60">
+        <v>394</v>
+      </c>
+      <c r="D19" s="23">
+        <v>1</v>
+      </c>
+      <c r="E19" s="23">
+        <v>2</v>
+      </c>
+      <c r="F19" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="23">
+        <v>17</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="C20" s="60">
+        <v>343</v>
+      </c>
+      <c r="D20" s="23">
+        <v>1</v>
+      </c>
+      <c r="E20" s="23">
+        <v>2</v>
+      </c>
+      <c r="F20" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="23">
+        <v>18</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="C21" s="60">
+        <v>298</v>
+      </c>
+      <c r="D21" s="23">
+        <v>1</v>
+      </c>
+      <c r="E21" s="23">
+        <v>2</v>
+      </c>
+      <c r="F21" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="23">
+        <v>19</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="C22" s="60">
+        <v>265</v>
+      </c>
+      <c r="D22" s="23">
+        <v>1</v>
+      </c>
+      <c r="E22" s="23">
+        <v>2</v>
+      </c>
+      <c r="F22" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="23">
+        <v>20</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="C23" s="60">
+        <v>183</v>
+      </c>
+      <c r="D23" s="23">
+        <v>1</v>
+      </c>
+      <c r="E23" s="23">
+        <v>2</v>
+      </c>
+      <c r="F23" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="23">
+        <v>21</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="C24" s="60">
+        <v>94</v>
+      </c>
+      <c r="D24" s="23">
+        <v>1</v>
+      </c>
+      <c r="E24" s="23">
+        <v>2</v>
+      </c>
+      <c r="F24" s="23">
         <v>1</v>
       </c>
     </row>
@@ -1759,22 +2202,22 @@
         <v>19</v>
       </c>
       <c r="D3" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="G3" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="I3" s="4" t="s">
         <v>67</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
@@ -1782,7 +2225,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C4" s="23">
         <v>956</v>
@@ -1791,19 +2234,19 @@
         <v>0</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F4" s="25">
         <v>0</v>
       </c>
       <c r="G4" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H4" s="24">
         <v>956</v>
       </c>
       <c r="I4" s="23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
@@ -1811,7 +2254,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C5" s="23">
         <v>736</v>
@@ -1820,19 +2263,19 @@
         <v>736</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F5" s="25">
         <v>0</v>
       </c>
       <c r="G5" s="23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H5" s="25">
         <v>0</v>
       </c>
       <c r="I5" s="23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1876,165 +2319,165 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="59" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
     </row>
     <row r="2" spans="1:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="58" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="58"/>
+      <c r="M2" s="58"/>
+      <c r="N2" s="58"/>
+    </row>
+    <row r="3" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="49" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49"/>
-    </row>
-    <row r="3" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36" t="s">
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="34"/>
+    </row>
+    <row r="4" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="34"/>
+      <c r="C4" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="41"/>
+      <c r="L4" s="41"/>
+      <c r="M4" s="41"/>
+      <c r="N4" s="41"/>
+    </row>
+    <row r="5" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="36"/>
-      <c r="M3" s="36"/>
-      <c r="N3" s="36"/>
-    </row>
-    <row r="4" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="37"/>
-      <c r="M4" s="37"/>
-      <c r="N4" s="37"/>
-    </row>
-    <row r="5" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36" t="s">
-        <v>71</v>
-      </c>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36"/>
-      <c r="J5" s="36"/>
-      <c r="K5" s="36"/>
-      <c r="L5" s="36"/>
-      <c r="M5" s="36"/>
-      <c r="N5" s="36"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="34"/>
+      <c r="M5" s="34"/>
+      <c r="N5" s="34"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="50"/>
-      <c r="B6" s="50"/>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="50"/>
-      <c r="H6" s="50"/>
-      <c r="I6" s="50"/>
-      <c r="J6" s="50"/>
-      <c r="K6" s="50"/>
-      <c r="L6" s="50"/>
-      <c r="M6" s="50"/>
-      <c r="N6" s="50"/>
+      <c r="A6" s="57"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="57"/>
+      <c r="K6" s="57"/>
+      <c r="L6" s="57"/>
+      <c r="M6" s="57"/>
+      <c r="N6" s="57"/>
     </row>
     <row r="7" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="49" t="s">
+      <c r="A7" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="49"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="49"/>
-      <c r="J7" s="49"/>
-      <c r="K7" s="49"/>
-      <c r="L7" s="49"/>
-      <c r="M7" s="49"/>
-      <c r="N7" s="49"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="58"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="58"/>
+      <c r="J7" s="58"/>
+      <c r="K7" s="58"/>
+      <c r="L7" s="58"/>
+      <c r="M7" s="58"/>
+      <c r="N7" s="58"/>
     </row>
     <row r="8" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="36" t="s">
+      <c r="A8" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="36"/>
+      <c r="B8" s="34"/>
       <c r="C8" s="14" t="s">
         <v>46</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E8" s="16" t="s">
         <v>47</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G8" s="18" t="s">
         <v>48</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I8" s="19" t="s">
         <v>49</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K8" s="20" t="s">
         <v>50</v>
@@ -2046,203 +2489,220 @@
       <c r="N8" s="17"/>
     </row>
     <row r="9" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="B9" s="36"/>
-      <c r="C9" s="54" t="s">
+      <c r="B9" s="34"/>
+      <c r="C9" s="55" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" s="52"/>
+      <c r="E9" s="56" t="s">
         <v>75</v>
       </c>
-      <c r="D9" s="51"/>
-      <c r="E9" s="55" t="s">
-        <v>76</v>
-      </c>
-      <c r="F9" s="51"/>
-      <c r="G9" s="55" t="s">
-        <v>76</v>
-      </c>
-      <c r="H9" s="51"/>
-      <c r="I9" s="55" t="s">
-        <v>76</v>
-      </c>
-      <c r="J9" s="51"/>
-      <c r="K9" s="51"/>
-      <c r="L9" s="51"/>
-      <c r="M9" s="51"/>
-      <c r="N9" s="51"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="56" t="s">
+        <v>75</v>
+      </c>
+      <c r="H9" s="52"/>
+      <c r="I9" s="56" t="s">
+        <v>75</v>
+      </c>
+      <c r="J9" s="52"/>
+      <c r="K9" s="52"/>
+      <c r="L9" s="52"/>
+      <c r="M9" s="52"/>
+      <c r="N9" s="52"/>
     </row>
     <row r="10" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="36" t="s">
+      <c r="A10" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="36"/>
-      <c r="C10" s="52">
-        <v>1</v>
-      </c>
-      <c r="D10" s="52"/>
-      <c r="E10" s="53">
-        <v>1</v>
-      </c>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53">
-        <v>0</v>
-      </c>
-      <c r="H10" s="53"/>
-      <c r="I10" s="53">
-        <v>0</v>
-      </c>
-      <c r="J10" s="53"/>
-      <c r="K10" s="53"/>
-      <c r="L10" s="53"/>
-      <c r="M10" s="53"/>
-      <c r="N10" s="53"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="53">
+        <v>1</v>
+      </c>
+      <c r="D10" s="53"/>
+      <c r="E10" s="54">
+        <v>1</v>
+      </c>
+      <c r="F10" s="54"/>
+      <c r="G10" s="54">
+        <v>0</v>
+      </c>
+      <c r="H10" s="54"/>
+      <c r="I10" s="54">
+        <v>0</v>
+      </c>
+      <c r="J10" s="54"/>
+      <c r="K10" s="54"/>
+      <c r="L10" s="54"/>
+      <c r="M10" s="54"/>
+      <c r="N10" s="54"/>
     </row>
     <row r="11" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="36"/>
-      <c r="C11" s="56">
+      <c r="B11" s="34"/>
+      <c r="C11" s="49">
         <v>10.553000000000001</v>
       </c>
-      <c r="D11" s="56"/>
-      <c r="E11" s="56">
+      <c r="D11" s="49"/>
+      <c r="E11" s="49">
         <v>7.673</v>
       </c>
-      <c r="F11" s="56"/>
-      <c r="G11" s="56">
-        <v>0</v>
-      </c>
-      <c r="H11" s="56"/>
-      <c r="I11" s="56">
-        <v>0</v>
-      </c>
-      <c r="J11" s="56"/>
-      <c r="K11" s="56"/>
-      <c r="L11" s="56"/>
-      <c r="M11" s="56"/>
-      <c r="N11" s="56"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="49">
+        <v>0</v>
+      </c>
+      <c r="H11" s="49"/>
+      <c r="I11" s="49">
+        <v>0</v>
+      </c>
+      <c r="J11" s="49"/>
+      <c r="K11" s="49"/>
+      <c r="L11" s="49"/>
+      <c r="M11" s="49"/>
+      <c r="N11" s="49"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="57"/>
-      <c r="B12" s="57"/>
-      <c r="C12" s="57"/>
-      <c r="D12" s="57"/>
-      <c r="E12" s="57"/>
-      <c r="F12" s="57"/>
-      <c r="G12" s="57"/>
-      <c r="H12" s="57"/>
-      <c r="I12" s="57"/>
-      <c r="J12" s="57"/>
-      <c r="K12" s="57"/>
-      <c r="L12" s="57"/>
-      <c r="M12" s="57"/>
-      <c r="N12" s="57"/>
+      <c r="A12" s="50"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="50"/>
+      <c r="I12" s="50"/>
+      <c r="J12" s="50"/>
+      <c r="K12" s="50"/>
+      <c r="L12" s="50"/>
+      <c r="M12" s="50"/>
+      <c r="N12" s="50"/>
     </row>
     <row r="13" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="B13" s="35"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="35"/>
-      <c r="L13" s="35"/>
-      <c r="M13" s="35"/>
-      <c r="N13" s="35"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="39"/>
+      <c r="L13" s="39"/>
+      <c r="M13" s="39"/>
+      <c r="N13" s="39"/>
     </row>
     <row r="14" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="58" t="s">
+      <c r="A14" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="58" t="s">
+      <c r="B14" s="51" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="58" t="s">
+      <c r="C14" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="58"/>
-      <c r="E14" s="58" t="s">
+      <c r="D14" s="51"/>
+      <c r="E14" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="F14" s="58"/>
-      <c r="G14" s="58" t="s">
+      <c r="F14" s="51"/>
+      <c r="G14" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="H14" s="58"/>
-      <c r="I14" s="36" t="s">
+      <c r="H14" s="51"/>
+      <c r="I14" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="J14" s="36"/>
-      <c r="K14" s="36"/>
-      <c r="L14" s="36"/>
-      <c r="M14" s="36"/>
-      <c r="N14" s="36"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="34"/>
     </row>
     <row r="15" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="59" t="s">
+      <c r="A15" s="48" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" s="48"/>
+      <c r="C15" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="E15" s="48">
+        <v>0</v>
+      </c>
+      <c r="F15" s="48"/>
+      <c r="G15" s="48">
+        <v>0</v>
+      </c>
+      <c r="H15" s="48"/>
+      <c r="I15" s="48">
+        <v>7.673</v>
+      </c>
+      <c r="J15" s="48"/>
+    </row>
+    <row r="16" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="B15" s="59"/>
-      <c r="C15" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="D15" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="E15" s="59">
-        <v>0</v>
-      </c>
-      <c r="F15" s="59"/>
-      <c r="G15" s="59">
-        <v>0</v>
-      </c>
-      <c r="H15" s="59"/>
-      <c r="I15" s="59">
-        <v>7.673</v>
-      </c>
-      <c r="J15" s="59"/>
-    </row>
-    <row r="16" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="59" t="s">
-        <v>87</v>
-      </c>
-      <c r="B16" s="59"/>
+      <c r="B16" s="48"/>
       <c r="C16" s="27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="E16" s="59">
+        <v>69</v>
+      </c>
+      <c r="E16" s="48">
         <v>736</v>
       </c>
-      <c r="F16" s="59"/>
-      <c r="G16" s="59">
+      <c r="F16" s="48"/>
+      <c r="G16" s="48">
         <v>736</v>
       </c>
-      <c r="H16" s="59"/>
-      <c r="I16" s="59">
+      <c r="H16" s="48"/>
+      <c r="I16" s="48">
         <v>10.553000000000001</v>
       </c>
-      <c r="J16" s="59"/>
+      <c r="J16" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="B2:N2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:N3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:N4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:N5"/>
+    <mergeCell ref="A6:N6"/>
+    <mergeCell ref="A7:N7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
     <mergeCell ref="K11:L11"/>
     <mergeCell ref="M11:N11"/>
     <mergeCell ref="A12:N12"/>
@@ -2257,31 +2717,14 @@
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="I11:J11"/>
     <mergeCell ref="A14:B14"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:N5"/>
-    <mergeCell ref="A6:N6"/>
-    <mergeCell ref="A7:N7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B2:N2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:N3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:N4"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait"/>
@@ -2319,165 +2762,165 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="59" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
     </row>
     <row r="2" spans="1:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="58" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="58"/>
+      <c r="M2" s="58"/>
+      <c r="N2" s="58"/>
+    </row>
+    <row r="3" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="49" t="s">
-        <v>66</v>
-      </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49"/>
-    </row>
-    <row r="3" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="36"/>
-      <c r="M3" s="36"/>
-      <c r="N3" s="36"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="34"/>
     </row>
     <row r="4" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="37">
-        <v>0</v>
-      </c>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="37"/>
-      <c r="M4" s="37"/>
-      <c r="N4" s="37"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="41">
+        <v>0</v>
+      </c>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="41"/>
+      <c r="L4" s="41"/>
+      <c r="M4" s="41"/>
+      <c r="N4" s="41"/>
     </row>
     <row r="5" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36" t="s">
-        <v>71</v>
-      </c>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36"/>
-      <c r="J5" s="36"/>
-      <c r="K5" s="36"/>
-      <c r="L5" s="36"/>
-      <c r="M5" s="36"/>
-      <c r="N5" s="36"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="34"/>
+      <c r="M5" s="34"/>
+      <c r="N5" s="34"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="50"/>
-      <c r="B6" s="50"/>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="50"/>
-      <c r="H6" s="50"/>
-      <c r="I6" s="50"/>
-      <c r="J6" s="50"/>
-      <c r="K6" s="50"/>
-      <c r="L6" s="50"/>
-      <c r="M6" s="50"/>
-      <c r="N6" s="50"/>
+      <c r="A6" s="57"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="57"/>
+      <c r="K6" s="57"/>
+      <c r="L6" s="57"/>
+      <c r="M6" s="57"/>
+      <c r="N6" s="57"/>
     </row>
     <row r="7" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="49" t="s">
+      <c r="A7" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="49"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="49"/>
-      <c r="J7" s="49"/>
-      <c r="K7" s="49"/>
-      <c r="L7" s="49"/>
-      <c r="M7" s="49"/>
-      <c r="N7" s="49"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="58"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="58"/>
+      <c r="J7" s="58"/>
+      <c r="K7" s="58"/>
+      <c r="L7" s="58"/>
+      <c r="M7" s="58"/>
+      <c r="N7" s="58"/>
     </row>
     <row r="8" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="36" t="s">
+      <c r="A8" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="36"/>
+      <c r="B8" s="34"/>
       <c r="C8" s="14" t="s">
         <v>46</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E8" s="16" t="s">
         <v>47</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G8" s="18" t="s">
         <v>48</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I8" s="19" t="s">
         <v>49</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K8" s="20" t="s">
         <v>50</v>
@@ -2489,203 +2932,220 @@
       <c r="N8" s="17"/>
     </row>
     <row r="9" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="B9" s="36"/>
-      <c r="C9" s="54" t="s">
+      <c r="B9" s="34"/>
+      <c r="C9" s="55" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" s="52"/>
+      <c r="E9" s="56" t="s">
         <v>75</v>
       </c>
-      <c r="D9" s="51"/>
-      <c r="E9" s="55" t="s">
-        <v>76</v>
-      </c>
-      <c r="F9" s="51"/>
-      <c r="G9" s="55" t="s">
-        <v>76</v>
-      </c>
-      <c r="H9" s="51"/>
-      <c r="I9" s="55" t="s">
-        <v>76</v>
-      </c>
-      <c r="J9" s="51"/>
-      <c r="K9" s="51"/>
-      <c r="L9" s="51"/>
-      <c r="M9" s="51"/>
-      <c r="N9" s="51"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="56" t="s">
+        <v>75</v>
+      </c>
+      <c r="H9" s="52"/>
+      <c r="I9" s="56" t="s">
+        <v>75</v>
+      </c>
+      <c r="J9" s="52"/>
+      <c r="K9" s="52"/>
+      <c r="L9" s="52"/>
+      <c r="M9" s="52"/>
+      <c r="N9" s="52"/>
     </row>
     <row r="10" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="36" t="s">
+      <c r="A10" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="36"/>
-      <c r="C10" s="52">
-        <v>0</v>
-      </c>
-      <c r="D10" s="52"/>
-      <c r="E10" s="53">
-        <v>1</v>
-      </c>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53">
-        <v>1</v>
-      </c>
-      <c r="H10" s="53"/>
-      <c r="I10" s="53">
-        <v>0</v>
-      </c>
-      <c r="J10" s="53"/>
-      <c r="K10" s="53"/>
-      <c r="L10" s="53"/>
-      <c r="M10" s="53"/>
-      <c r="N10" s="53"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="53">
+        <v>0</v>
+      </c>
+      <c r="D10" s="53"/>
+      <c r="E10" s="54">
+        <v>1</v>
+      </c>
+      <c r="F10" s="54"/>
+      <c r="G10" s="54">
+        <v>1</v>
+      </c>
+      <c r="H10" s="54"/>
+      <c r="I10" s="54">
+        <v>0</v>
+      </c>
+      <c r="J10" s="54"/>
+      <c r="K10" s="54"/>
+      <c r="L10" s="54"/>
+      <c r="M10" s="54"/>
+      <c r="N10" s="54"/>
     </row>
     <row r="11" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="36"/>
-      <c r="C11" s="56">
-        <v>0</v>
-      </c>
-      <c r="D11" s="56"/>
-      <c r="E11" s="56">
+      <c r="B11" s="34"/>
+      <c r="C11" s="49">
+        <v>0</v>
+      </c>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49">
         <v>7.9020000000000001</v>
       </c>
-      <c r="F11" s="56"/>
-      <c r="G11" s="56">
+      <c r="F11" s="49"/>
+      <c r="G11" s="49">
         <v>3.0590000000000002</v>
       </c>
-      <c r="H11" s="56"/>
-      <c r="I11" s="56">
-        <v>0</v>
-      </c>
-      <c r="J11" s="56"/>
-      <c r="K11" s="56"/>
-      <c r="L11" s="56"/>
-      <c r="M11" s="56"/>
-      <c r="N11" s="56"/>
+      <c r="H11" s="49"/>
+      <c r="I11" s="49">
+        <v>0</v>
+      </c>
+      <c r="J11" s="49"/>
+      <c r="K11" s="49"/>
+      <c r="L11" s="49"/>
+      <c r="M11" s="49"/>
+      <c r="N11" s="49"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="57"/>
-      <c r="B12" s="57"/>
-      <c r="C12" s="57"/>
-      <c r="D12" s="57"/>
-      <c r="E12" s="57"/>
-      <c r="F12" s="57"/>
-      <c r="G12" s="57"/>
-      <c r="H12" s="57"/>
-      <c r="I12" s="57"/>
-      <c r="J12" s="57"/>
-      <c r="K12" s="57"/>
-      <c r="L12" s="57"/>
-      <c r="M12" s="57"/>
-      <c r="N12" s="57"/>
+      <c r="A12" s="50"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="50"/>
+      <c r="I12" s="50"/>
+      <c r="J12" s="50"/>
+      <c r="K12" s="50"/>
+      <c r="L12" s="50"/>
+      <c r="M12" s="50"/>
+      <c r="N12" s="50"/>
     </row>
     <row r="13" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="B13" s="35"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="35"/>
-      <c r="L13" s="35"/>
-      <c r="M13" s="35"/>
-      <c r="N13" s="35"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="39"/>
+      <c r="L13" s="39"/>
+      <c r="M13" s="39"/>
+      <c r="N13" s="39"/>
     </row>
     <row r="14" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="58" t="s">
+      <c r="A14" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="58" t="s">
+      <c r="B14" s="51" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="58" t="s">
+      <c r="C14" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="58"/>
-      <c r="E14" s="58" t="s">
+      <c r="D14" s="51"/>
+      <c r="E14" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="F14" s="58"/>
-      <c r="G14" s="58" t="s">
+      <c r="F14" s="51"/>
+      <c r="G14" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="H14" s="58"/>
-      <c r="I14" s="36" t="s">
+      <c r="H14" s="51"/>
+      <c r="I14" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="J14" s="36"/>
-      <c r="K14" s="36"/>
-      <c r="L14" s="36"/>
-      <c r="M14" s="36"/>
-      <c r="N14" s="36"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="34"/>
     </row>
     <row r="15" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="59" t="s">
+      <c r="A15" s="48" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" s="48"/>
+      <c r="C15" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="E15" s="48">
+        <v>0</v>
+      </c>
+      <c r="F15" s="48"/>
+      <c r="G15" s="48">
+        <v>0</v>
+      </c>
+      <c r="H15" s="48"/>
+      <c r="I15" s="48">
+        <v>3.0590000000000002</v>
+      </c>
+      <c r="J15" s="48"/>
+    </row>
+    <row r="16" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="B15" s="59"/>
-      <c r="C15" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="D15" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="E15" s="59">
-        <v>0</v>
-      </c>
-      <c r="F15" s="59"/>
-      <c r="G15" s="59">
-        <v>0</v>
-      </c>
-      <c r="H15" s="59"/>
-      <c r="I15" s="59">
-        <v>3.0590000000000002</v>
-      </c>
-      <c r="J15" s="59"/>
-    </row>
-    <row r="16" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="59" t="s">
-        <v>87</v>
-      </c>
-      <c r="B16" s="59"/>
+      <c r="B16" s="48"/>
       <c r="C16" s="29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>79</v>
-      </c>
-      <c r="E16" s="59">
-        <v>0</v>
-      </c>
-      <c r="F16" s="59"/>
-      <c r="G16" s="59">
+        <v>78</v>
+      </c>
+      <c r="E16" s="48">
+        <v>0</v>
+      </c>
+      <c r="F16" s="48"/>
+      <c r="G16" s="48">
         <v>736</v>
       </c>
-      <c r="H16" s="59"/>
-      <c r="I16" s="59">
+      <c r="H16" s="48"/>
+      <c r="I16" s="48">
         <v>7.9020000000000001</v>
       </c>
-      <c r="J16" s="59"/>
+      <c r="J16" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="B2:N2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:N3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:N4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:N5"/>
+    <mergeCell ref="A6:N6"/>
+    <mergeCell ref="A7:N7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
     <mergeCell ref="K11:L11"/>
     <mergeCell ref="M11:N11"/>
     <mergeCell ref="A12:N12"/>
@@ -2700,31 +3160,14 @@
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="I11:J11"/>
     <mergeCell ref="A14:B14"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:N5"/>
-    <mergeCell ref="A6:N6"/>
-    <mergeCell ref="A7:N7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B2:N2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:N3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:N4"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait"/>
@@ -2762,165 +3205,165 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="59" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
     </row>
     <row r="2" spans="1:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="58" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="58"/>
+      <c r="M2" s="58"/>
+      <c r="N2" s="58"/>
+    </row>
+    <row r="3" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="49" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49"/>
-    </row>
-    <row r="3" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36" t="s">
-        <v>82</v>
-      </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="36"/>
-      <c r="M3" s="36"/>
-      <c r="N3" s="36"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="34"/>
     </row>
     <row r="4" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="37">
+      <c r="B4" s="34"/>
+      <c r="C4" s="41">
         <v>0.5</v>
       </c>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="37"/>
-      <c r="M4" s="37"/>
-      <c r="N4" s="37"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="41"/>
+      <c r="L4" s="41"/>
+      <c r="M4" s="41"/>
+      <c r="N4" s="41"/>
     </row>
     <row r="5" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36" t="s">
-        <v>71</v>
-      </c>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36"/>
-      <c r="J5" s="36"/>
-      <c r="K5" s="36"/>
-      <c r="L5" s="36"/>
-      <c r="M5" s="36"/>
-      <c r="N5" s="36"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="34"/>
+      <c r="M5" s="34"/>
+      <c r="N5" s="34"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="50"/>
-      <c r="B6" s="50"/>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="50"/>
-      <c r="H6" s="50"/>
-      <c r="I6" s="50"/>
-      <c r="J6" s="50"/>
-      <c r="K6" s="50"/>
-      <c r="L6" s="50"/>
-      <c r="M6" s="50"/>
-      <c r="N6" s="50"/>
+      <c r="A6" s="57"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="57"/>
+      <c r="K6" s="57"/>
+      <c r="L6" s="57"/>
+      <c r="M6" s="57"/>
+      <c r="N6" s="57"/>
     </row>
     <row r="7" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="49" t="s">
+      <c r="A7" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="49"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="49"/>
-      <c r="J7" s="49"/>
-      <c r="K7" s="49"/>
-      <c r="L7" s="49"/>
-      <c r="M7" s="49"/>
-      <c r="N7" s="49"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="58"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="58"/>
+      <c r="J7" s="58"/>
+      <c r="K7" s="58"/>
+      <c r="L7" s="58"/>
+      <c r="M7" s="58"/>
+      <c r="N7" s="58"/>
     </row>
     <row r="8" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="36" t="s">
+      <c r="A8" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="36"/>
+      <c r="B8" s="34"/>
       <c r="C8" s="14" t="s">
         <v>46</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E8" s="16" t="s">
         <v>47</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G8" s="18" t="s">
         <v>48</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I8" s="19" t="s">
         <v>49</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K8" s="20" t="s">
         <v>50</v>
@@ -2932,203 +3375,220 @@
       <c r="N8" s="17"/>
     </row>
     <row r="9" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="B9" s="36"/>
-      <c r="C9" s="54" t="s">
+      <c r="B9" s="34"/>
+      <c r="C9" s="55" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" s="52"/>
+      <c r="E9" s="56" t="s">
         <v>75</v>
       </c>
-      <c r="D9" s="51"/>
-      <c r="E9" s="55" t="s">
-        <v>76</v>
-      </c>
-      <c r="F9" s="51"/>
-      <c r="G9" s="55" t="s">
-        <v>76</v>
-      </c>
-      <c r="H9" s="51"/>
-      <c r="I9" s="55" t="s">
-        <v>76</v>
-      </c>
-      <c r="J9" s="51"/>
-      <c r="K9" s="51"/>
-      <c r="L9" s="51"/>
-      <c r="M9" s="51"/>
-      <c r="N9" s="51"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="56" t="s">
+        <v>75</v>
+      </c>
+      <c r="H9" s="52"/>
+      <c r="I9" s="56" t="s">
+        <v>75</v>
+      </c>
+      <c r="J9" s="52"/>
+      <c r="K9" s="52"/>
+      <c r="L9" s="52"/>
+      <c r="M9" s="52"/>
+      <c r="N9" s="52"/>
     </row>
     <row r="10" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="36" t="s">
+      <c r="A10" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="36"/>
-      <c r="C10" s="52">
-        <v>1</v>
-      </c>
-      <c r="D10" s="52"/>
-      <c r="E10" s="53">
-        <v>0</v>
-      </c>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53">
-        <v>1</v>
-      </c>
-      <c r="H10" s="53"/>
-      <c r="I10" s="53">
-        <v>0</v>
-      </c>
-      <c r="J10" s="53"/>
-      <c r="K10" s="53"/>
-      <c r="L10" s="53"/>
-      <c r="M10" s="53"/>
-      <c r="N10" s="53"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="53">
+        <v>1</v>
+      </c>
+      <c r="D10" s="53"/>
+      <c r="E10" s="54">
+        <v>0</v>
+      </c>
+      <c r="F10" s="54"/>
+      <c r="G10" s="54">
+        <v>1</v>
+      </c>
+      <c r="H10" s="54"/>
+      <c r="I10" s="54">
+        <v>0</v>
+      </c>
+      <c r="J10" s="54"/>
+      <c r="K10" s="54"/>
+      <c r="L10" s="54"/>
+      <c r="M10" s="54"/>
+      <c r="N10" s="54"/>
     </row>
     <row r="11" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="36"/>
-      <c r="C11" s="56">
+      <c r="B11" s="34"/>
+      <c r="C11" s="49">
         <v>1.766</v>
       </c>
-      <c r="D11" s="56"/>
-      <c r="E11" s="56">
-        <v>0</v>
-      </c>
-      <c r="F11" s="56"/>
-      <c r="G11" s="56">
+      <c r="D11" s="49"/>
+      <c r="E11" s="49">
+        <v>0</v>
+      </c>
+      <c r="F11" s="49"/>
+      <c r="G11" s="49">
         <v>6.391</v>
       </c>
-      <c r="H11" s="56"/>
-      <c r="I11" s="56">
-        <v>0</v>
-      </c>
-      <c r="J11" s="56"/>
-      <c r="K11" s="56"/>
-      <c r="L11" s="56"/>
-      <c r="M11" s="56"/>
-      <c r="N11" s="56"/>
+      <c r="H11" s="49"/>
+      <c r="I11" s="49">
+        <v>0</v>
+      </c>
+      <c r="J11" s="49"/>
+      <c r="K11" s="49"/>
+      <c r="L11" s="49"/>
+      <c r="M11" s="49"/>
+      <c r="N11" s="49"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="57"/>
-      <c r="B12" s="57"/>
-      <c r="C12" s="57"/>
-      <c r="D12" s="57"/>
-      <c r="E12" s="57"/>
-      <c r="F12" s="57"/>
-      <c r="G12" s="57"/>
-      <c r="H12" s="57"/>
-      <c r="I12" s="57"/>
-      <c r="J12" s="57"/>
-      <c r="K12" s="57"/>
-      <c r="L12" s="57"/>
-      <c r="M12" s="57"/>
-      <c r="N12" s="57"/>
+      <c r="A12" s="50"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="50"/>
+      <c r="I12" s="50"/>
+      <c r="J12" s="50"/>
+      <c r="K12" s="50"/>
+      <c r="L12" s="50"/>
+      <c r="M12" s="50"/>
+      <c r="N12" s="50"/>
     </row>
     <row r="13" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="B13" s="35"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="35"/>
-      <c r="L13" s="35"/>
-      <c r="M13" s="35"/>
-      <c r="N13" s="35"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="39"/>
+      <c r="L13" s="39"/>
+      <c r="M13" s="39"/>
+      <c r="N13" s="39"/>
     </row>
     <row r="14" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="58" t="s">
+      <c r="A14" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="58" t="s">
+      <c r="B14" s="51" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="58" t="s">
+      <c r="C14" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="58"/>
-      <c r="E14" s="58" t="s">
+      <c r="D14" s="51"/>
+      <c r="E14" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="F14" s="58"/>
-      <c r="G14" s="58" t="s">
+      <c r="F14" s="51"/>
+      <c r="G14" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="H14" s="58"/>
-      <c r="I14" s="36" t="s">
+      <c r="H14" s="51"/>
+      <c r="I14" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="J14" s="36"/>
-      <c r="K14" s="36"/>
-      <c r="L14" s="36"/>
-      <c r="M14" s="36"/>
-      <c r="N14" s="36"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="34"/>
     </row>
     <row r="15" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="59" t="s">
+      <c r="A15" s="48" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" s="48"/>
+      <c r="C15" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="E15" s="48">
+        <v>956</v>
+      </c>
+      <c r="F15" s="48"/>
+      <c r="G15" s="48">
+        <v>956</v>
+      </c>
+      <c r="H15" s="48"/>
+      <c r="I15" s="48">
+        <v>1.766</v>
+      </c>
+      <c r="J15" s="48"/>
+    </row>
+    <row r="16" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="B15" s="59"/>
-      <c r="C15" s="30" t="s">
+      <c r="B16" s="48"/>
+      <c r="C16" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="D15" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="E15" s="59">
-        <v>956</v>
-      </c>
-      <c r="F15" s="59"/>
-      <c r="G15" s="59">
-        <v>956</v>
-      </c>
-      <c r="H15" s="59"/>
-      <c r="I15" s="59">
-        <v>1.766</v>
-      </c>
-      <c r="J15" s="59"/>
-    </row>
-    <row r="16" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="59" t="s">
-        <v>87</v>
-      </c>
-      <c r="B16" s="59"/>
-      <c r="C16" s="31" t="s">
-        <v>76</v>
-      </c>
       <c r="D16" s="26" t="s">
-        <v>84</v>
-      </c>
-      <c r="E16" s="59">
-        <v>0</v>
-      </c>
-      <c r="F16" s="59"/>
-      <c r="G16" s="59">
+        <v>83</v>
+      </c>
+      <c r="E16" s="48">
+        <v>0</v>
+      </c>
+      <c r="F16" s="48"/>
+      <c r="G16" s="48">
         <v>736</v>
       </c>
-      <c r="H16" s="59"/>
-      <c r="I16" s="59">
+      <c r="H16" s="48"/>
+      <c r="I16" s="48">
         <v>6.391</v>
       </c>
-      <c r="J16" s="59"/>
+      <c r="J16" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="B2:N2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:N3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:N4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:N5"/>
+    <mergeCell ref="A6:N6"/>
+    <mergeCell ref="A7:N7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
     <mergeCell ref="K11:L11"/>
     <mergeCell ref="M11:N11"/>
     <mergeCell ref="A12:N12"/>
@@ -3143,31 +3603,14 @@
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="I11:J11"/>
     <mergeCell ref="A14:B14"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:N5"/>
-    <mergeCell ref="A6:N6"/>
-    <mergeCell ref="A7:N7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B2:N2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:N3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:N4"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait"/>
@@ -3269,36 +3712,36 @@
     </row>
     <row r="2" spans="1:20" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>70</v>
-      </c>
       <c r="D2" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="F2" s="22" t="s">
         <v>73</v>
-      </c>
-      <c r="F2" s="22" t="s">
-        <v>74</v>
       </c>
       <c r="G2" s="22"/>
       <c r="H2" s="22"/>
       <c r="I2" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J2" s="23">
         <v>20</v>
       </c>
       <c r="K2" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L2" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M2" s="22" t="s">
         <v>35</v>
@@ -3319,7 +3762,7 @@
         <v>0</v>
       </c>
       <c r="S2" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="T2" s="23">
         <v>7.673</v>
@@ -3327,36 +3770,36 @@
     </row>
     <row r="3" spans="1:20" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>70</v>
-      </c>
       <c r="D3" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="F3" s="22" t="s">
         <v>73</v>
-      </c>
-      <c r="F3" s="22" t="s">
-        <v>74</v>
       </c>
       <c r="G3" s="22"/>
       <c r="H3" s="22"/>
       <c r="I3" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J3" s="23">
         <v>20</v>
       </c>
       <c r="K3" s="22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L3" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M3" s="22" t="s">
         <v>34</v>
@@ -3377,7 +3820,7 @@
         <v>736</v>
       </c>
       <c r="S3" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="T3" s="23">
         <v>10.553000000000001</v>
@@ -3385,36 +3828,36 @@
     </row>
     <row r="4" spans="1:20" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="B4" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="C4" s="22" t="s">
+      <c r="D4" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="E4" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F4" s="22" t="s">
         <v>79</v>
-      </c>
-      <c r="E4" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="F4" s="22" t="s">
-        <v>80</v>
       </c>
       <c r="G4" s="22"/>
       <c r="H4" s="22"/>
       <c r="I4" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J4" s="23">
         <v>20</v>
       </c>
       <c r="K4" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L4" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M4" s="22" t="s">
         <v>35</v>
@@ -3435,7 +3878,7 @@
         <v>0</v>
       </c>
       <c r="S4" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="T4" s="23">
         <v>3.0590000000000002</v>
@@ -3443,36 +3886,36 @@
     </row>
     <row r="5" spans="1:20" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="B5" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="C5" s="22" t="s">
+      <c r="D5" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="E5" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5" s="22" t="s">
         <v>79</v>
-      </c>
-      <c r="E5" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="F5" s="22" t="s">
-        <v>80</v>
       </c>
       <c r="G5" s="22"/>
       <c r="H5" s="22"/>
       <c r="I5" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J5" s="23">
         <v>20</v>
       </c>
       <c r="K5" s="22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L5" s="22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M5" s="22" t="s">
         <v>35</v>
@@ -3493,7 +3936,7 @@
         <v>736</v>
       </c>
       <c r="S5" s="23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="T5" s="23">
         <v>7.9020000000000001</v>
@@ -3501,36 +3944,36 @@
     </row>
     <row r="6" spans="1:20" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="B6" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="C6" s="22" t="s">
+      <c r="D6" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="E6" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="F6" s="22" t="s">
         <v>84</v>
-      </c>
-      <c r="F6" s="22" t="s">
-        <v>85</v>
       </c>
       <c r="G6" s="22"/>
       <c r="H6" s="22"/>
       <c r="I6" s="22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J6" s="23">
         <v>20</v>
       </c>
       <c r="K6" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L6" s="22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M6" s="22" t="s">
         <v>34</v>
@@ -3551,7 +3994,7 @@
         <v>956</v>
       </c>
       <c r="S6" s="23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="T6" s="23">
         <v>1.766</v>
@@ -3559,36 +4002,36 @@
     </row>
     <row r="7" spans="1:20" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="B7" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="C7" s="22" t="s">
+      <c r="D7" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="E7" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="F7" s="22" t="s">
         <v>84</v>
-      </c>
-      <c r="F7" s="22" t="s">
-        <v>85</v>
       </c>
       <c r="G7" s="22"/>
       <c r="H7" s="22"/>
       <c r="I7" s="22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J7" s="23">
         <v>20</v>
       </c>
       <c r="K7" s="22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L7" s="22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M7" s="22" t="s">
         <v>35</v>
@@ -3609,7 +4052,7 @@
         <v>736</v>
       </c>
       <c r="S7" s="23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="T7" s="23">
         <v>6.391</v>

</xml_diff>